<commit_message>
update fetch api in MainActivity.
</commit_message>
<xml_diff>
--- a/docs/mapping_1.xlsx
+++ b/docs/mapping_1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{64DBC902-9248-42B5-B241-B154A5F5B0EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{616AB6FF-5121-45EB-BF13-DB684AC39333}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="料盒动作地址" sheetId="4" r:id="rId1"/>
@@ -3428,8 +3428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895E1E7A-D55B-4209-9AA8-8C47268BF6B5}">
   <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5088,7 +5088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD35890-9E09-48E1-AAD0-F3433AB7274A}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -5538,8 +5538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282B03E3-F049-4FAE-B767-B79205C70F1F}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5929,7 +5929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED724FD2-37F6-4369-979A-69881B916AA8}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -6814,12 +6814,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="A20:A27"/>
-    <mergeCell ref="D21:D23"/>
     <mergeCell ref="A56:A59"/>
     <mergeCell ref="D57:D58"/>
     <mergeCell ref="A29:A36"/>
@@ -6828,6 +6822,12 @@
     <mergeCell ref="D39:D41"/>
     <mergeCell ref="A47:A54"/>
     <mergeCell ref="D48:D50"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="D21:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6837,7 +6837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F88D21D-F4C2-4C8F-821D-4730A620D578}">
   <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>